<commit_message>
updated results with DeepEval Contextual Precision metric run for Gemini 2.0 Exp
</commit_message>
<xml_diff>
--- a/results/LibraryComparisonChart.xlsx
+++ b/results/LibraryComparisonChart.xlsx
@@ -263,7 +263,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -359,6 +359,9 @@
       <c r="B12" s="0" t="n">
         <v>0.967882</v>
       </c>
+      <c r="C12" s="0" t="n">
+        <v>0.756079</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">

</xml_diff>

<commit_message>
updated deepeval and ragas libraries to latest versions, updated results
</commit_message>
<xml_diff>
--- a/results/LibraryComparisonChart.xlsx
+++ b/results/LibraryComparisonChart.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t xml:space="preserve">Dataset: First 903 examples of datasets/rag_mini_wikipedia_complete_chat.csv</t>
   </si>
@@ -59,6 +59,36 @@
   </si>
   <si>
     <t xml:space="preserve">x (LLM; result calculated from PPI &amp; validation set accuracy- “Context Relevance”)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library Update Comparison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All using Gemini Flash 1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First 100 examples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contextual Precision (without reference)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avg # API Requests Per Example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAGAS v0.1.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAGAS v0.2.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contextual Precision (with reference)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DeepEval v1.1.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DeepEval v2.2.7</t>
   </si>
 </sst>
 </file>
@@ -260,14 +290,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="67.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.3"/>
@@ -351,6 +382,9 @@
       <c r="A11" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="B11" s="0" t="n">
+        <v>0.888797804643783</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -419,6 +453,79 @@
       </c>
       <c r="C18" s="0" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>0.747038558152573</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>0.711863888840233</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>0.796861</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added deepeval v2 2 7 results for comparison
</commit_message>
<xml_diff>
--- a/results/LibraryComparisonChart.xlsx
+++ b/results/LibraryComparisonChart.xlsx
@@ -98,7 +98,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -118,6 +118,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -162,9 +168,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -293,7 +303,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -523,9 +533,12 @@
         <v>0.796861</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>22</v>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>0.808914</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
continued analysis of results
</commit_message>
<xml_diff>
--- a/results/LibraryComparisonChart.xlsx
+++ b/results/LibraryComparisonChart.xlsx
@@ -98,8 +98,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -165,12 +166,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -299,8 +304,8 @@
   </sheetPr>
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -337,10 +342,10 @@
       <c r="A5" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>0.866768124469819</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>0.771483724377512</v>
       </c>
     </row>
@@ -348,10 +353,10 @@
       <c r="A6" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>0.958</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>0.792454</v>
       </c>
     </row>
@@ -359,10 +364,10 @@
       <c r="A7" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>0.692</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>0.711</v>
       </c>
       <c r="D7" s="0" t="n">
@@ -389,10 +394,10 @@
       <c r="A11" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>0.888797804643783</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>0.772337367384857</v>
       </c>
     </row>
@@ -400,10 +405,10 @@
       <c r="A12" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>0.967882</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>0.756079</v>
       </c>
     </row>
@@ -411,10 +416,10 @@
       <c r="A13" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>0.792</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>0.852</v>
       </c>
       <c r="D13" s="0" t="n">
@@ -492,7 +497,7 @@
       <c r="A25" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="1" t="n">
         <v>0.747038558152573</v>
       </c>
       <c r="C25" s="0" t="n">
@@ -503,7 +508,7 @@
       <c r="A26" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="1" t="n">
         <v>0.711863888840233</v>
       </c>
       <c r="C26" s="0" t="n">
@@ -519,6 +524,9 @@
       <c r="A28" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="C28" s="0" t="n">
+        <v>12.7</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
@@ -529,7 +537,7 @@
       <c r="A30" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="1" t="n">
         <v>0.796861</v>
       </c>
       <c r="C30" s="0" t="n">
@@ -540,7 +548,7 @@
       <c r="A31" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="1" t="n">
+      <c r="B31" s="2" t="n">
         <v>0.808914</v>
       </c>
       <c r="C31" s="0" t="n">

</xml_diff>

<commit_message>
updated with full analysis of all results
</commit_message>
<xml_diff>
--- a/results/LibraryComparisonChart.xlsx
+++ b/results/LibraryComparisonChart.xlsx
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
   <si>
     <t xml:space="preserve">Dataset: First 903 examples of datasets/rag_mini_wikipedia_complete_chat.csv</t>
   </si>
   <si>
-    <t xml:space="preserve">Gemini 1.5</t>
+    <t xml:space="preserve">LLM Judge: Gemini 1.5</t>
   </si>
   <si>
     <t xml:space="preserve">Faithfulness</t>
@@ -46,22 +46,22 @@
     <t xml:space="preserve">ARES</t>
   </si>
   <si>
-    <t xml:space="preserve">Gemini 2.0 Experimental</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x (LLM then # truthful claims / total # claims)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x (LLM request for each context node then weighted cumulative precision)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X (1 LLM request for all context nodes then weighted cumulative precision)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x (LLM; result calculated from PPI &amp; validation set accuracy)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x (LLM; result calculated from PPI &amp; validation set accuracy- “Context Relevance”)</t>
+    <t xml:space="preserve">LLM Judge: Gemini 2.0 Experimental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLM to extract and classify claims; then # truthful claims / total # claims</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLM request for each context node then weighted cumulative precision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 LLM request for all context nodes then weighted cumulative precision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLM; result calculated from PPI &amp; validation set accuracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLM; result calculated from PPI &amp; validation set accuracy- “Context Relevance”</t>
   </si>
   <si>
     <t xml:space="preserve">Library Update Comparison</t>
@@ -92,15 +92,31 @@
   </si>
   <si>
     <t xml:space="preserve">DeepEval v2.2.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average Difference between LLM Results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average Difference between Examples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAGAS and DeepEval, Gemini 1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAGAS and DeepEval, Gemini 2.0 Exp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of Examples within 0.1 scores of each other</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -166,7 +182,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -177,6 +193,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -302,17 +322,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="52.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="67.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.12"/>
   </cols>
@@ -433,9 +453,6 @@
       <c r="C15" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
@@ -524,6 +541,9 @@
       <c r="A28" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="B28" s="1" t="n">
+        <v>0.745486278078553</v>
+      </c>
       <c r="C28" s="0" t="n">
         <v>12.7</v>
       </c>
@@ -553,6 +573,113 @@
       </c>
       <c r="C31" s="0" t="n">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>0.077</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>0.069</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>0.054</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>0.145</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="1" t="n">
+        <v>0.161216071534399</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>0.172519308304842</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" s="1" t="n">
+        <v>0.122093926909796</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>0.183165000802064</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="3" t="n">
+        <f aca="false">640/903</f>
+        <v>0.70874861572536</v>
+      </c>
+      <c r="C45" s="3" t="n">
+        <f aca="false">525/903</f>
+        <v>0.581395348837209</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="3" t="n">
+        <f aca="false">709/903</f>
+        <v>0.78516057585825</v>
+      </c>
+      <c r="C46" s="3" t="n">
+        <f aca="false">506/903</f>
+        <v>0.560354374307863</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated chart with differences across results
</commit_message>
<xml_diff>
--- a/results/LibraryComparisonChart.xlsx
+++ b/results/LibraryComparisonChart.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t xml:space="preserve">Dataset: First 903 examples of datasets/rag_mini_wikipedia_complete_chat.csv</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">LLM Judge: Gemini 2.0 Experimental</t>
   </si>
   <si>
+    <t xml:space="preserve">Difference in results across LLMs-as-a-Judge:</t>
+  </si>
+  <si>
     <t xml:space="preserve">LLM to extract and classify claims; then # truthful claims / total # claims</t>
   </si>
   <si>
@@ -86,6 +89,9 @@
   </si>
   <si>
     <t xml:space="preserve">Contextual Precision (with reference)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Note: without rate-limiting errors, should be 10)</t>
   </si>
   <si>
     <t xml:space="preserve">DeepEval v1.1.6</t>
@@ -322,10 +328,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -447,237 +453,303 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+      <c r="A15" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C16" s="0" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>10</v>
+      <c r="D16" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <f aca="false">ABS(B11-B5)</f>
+        <v>0.022029680173964</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <f aca="false">ABS(C11-C5)</f>
+        <v>0.000853643007345029</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <f aca="false">ABS(B12-B6)</f>
+        <v>0.00988200000000006</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <f aca="false">ABS(C12-C6)</f>
+        <v>0.036375</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>13</v>
-      </c>
+      <c r="B19" s="1" t="n">
+        <f aca="false">ABS(B13-B7)</f>
+        <v>0.1</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <f aca="false">ABS(C13-C7)</f>
+        <v>0.141</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <f aca="false">ABS(D13-D7)</f>
+        <v>0.0850000000000001</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>14</v>
+      <c r="B21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>15</v>
+        <v>5</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>7</v>
+      </c>
       <c r="B24" s="0" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="1" t="n">
-        <v>0.747038558152573</v>
-      </c>
-      <c r="C25" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="1" t="n">
-        <v>0.711863888840233</v>
-      </c>
-      <c r="C26" s="0" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
-        <v>21</v>
+      <c r="A27" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="1" t="n">
+      <c r="B31" s="1" t="n">
+        <v>0.747038558152573</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="1" t="n">
+        <v>0.711863888840233</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="1" t="n">
         <v>0.745486278078553</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C34" s="0" t="n">
         <v>12.7</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="D34" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="B30" s="1" t="n">
-        <v>0.796861</v>
-      </c>
-      <c r="C30" s="0" t="n">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="2" t="n">
-        <v>0.808914</v>
-      </c>
-      <c r="C31" s="0" t="n">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" s="0" t="n">
-        <v>0.077</v>
-      </c>
-      <c r="C35" s="0" t="n">
-        <v>0.069</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="0" t="n">
-        <v>0.054</v>
+        <v>24</v>
+      </c>
+      <c r="B36" s="1" t="n">
+        <v>0.796861</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>0.145</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="2" t="n">
+        <v>0.808914</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="1" t="n">
-        <v>0.161216071534399</v>
-      </c>
-      <c r="C40" s="1" t="n">
-        <v>0.172519308304842</v>
+      <c r="B40" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B41" s="1" t="n">
-        <v>0.122093926909796</v>
-      </c>
-      <c r="C41" s="1" t="n">
-        <v>0.183165000802064</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>0.077</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>0.069</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>0.054</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>0.145</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C44" s="0" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B45" s="3" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46" s="1" t="n">
+        <v>0.161216071534399</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>0.172519308304842</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" s="1" t="n">
+        <v>0.122093926909796</v>
+      </c>
+      <c r="C47" s="1" t="n">
+        <v>0.183165000802064</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B51" s="3" t="n">
         <f aca="false">640/903</f>
         <v>0.70874861572536</v>
       </c>
-      <c r="C45" s="3" t="n">
+      <c r="C51" s="3" t="n">
         <f aca="false">525/903</f>
         <v>0.581395348837209</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B46" s="3" t="n">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52" s="3" t="n">
         <f aca="false">709/903</f>
         <v>0.78516057585825</v>
       </c>
-      <c r="C46" s="3" t="n">
+      <c r="C52" s="3" t="n">
         <f aca="false">506/903</f>
         <v>0.560354374307863</v>
       </c>

</xml_diff>